<commit_message>
try to fix fisher
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofia/PycharmProjects/WinPOC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\PycharmProjects\WinPOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB120CB-7D21-3746-B4FE-057DF38E0EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB24B85-4AD9-43A0-AE4C-D8A1BCD1ACAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
@@ -133,19 +133,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -464,191 +460,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
         <v>7</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D3" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6">
         <v>10</v>
       </c>
-      <c r="C3" s="8">
+      <c r="D4" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7">
         <v>10</v>
       </c>
-      <c r="D4" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8">
-        <v>8</v>
-      </c>
-      <c r="D5" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8">
-        <v>9</v>
-      </c>
-      <c r="D6" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="8">
-        <v>8</v>
-      </c>
-      <c r="D7" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>